<commit_message>
1) Muitas correções p/ validar e gravar os beneficiários;
</commit_message>
<xml_diff>
--- a/CoParticipacaoWebService/src/test/resources/marjan/output/NAO-LOCALIZADO-MARJAN-201806.xlsx
+++ b/CoParticipacaoWebService/src/test/resources/marjan/output/NAO-LOCALIZADO-MARJAN-201806.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DROXTER" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t xml:space="preserve">MATRICULA</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">MATRICULA EMPRESA</t>
   </si>
   <si>
-    <t xml:space="preserve">NOME DEPENDENTE</t>
+    <t xml:space="preserve">NOME BENEFICIÁRIO</t>
   </si>
   <si>
     <t xml:space="preserve">CPF</t>
@@ -40,21 +40,33 @@
     <t xml:space="preserve">VALOR PRINCIPAL</t>
   </si>
   <si>
+    <t xml:space="preserve">ANDRESSA RODRIGUES DE ARAUJO</t>
+  </si>
+  <si>
     <t xml:space="preserve">GUSTAVO GARCIA DE OLIVEIRA LIMA</t>
   </si>
   <si>
+    <t xml:space="preserve">LARISSA GEOVANA DOS SANTOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">LORENZO GARCIA DE OLIVEIRA LIMA</t>
   </si>
   <si>
     <t xml:space="preserve">MARIA AGUIDA MORAIS SOBRINHO</t>
   </si>
   <si>
+    <t xml:space="preserve">BEATRIZ GUIMARAES BORGES</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLAUDIA ALEXANDRA MARTINS ROMAR</t>
   </si>
   <si>
     <t xml:space="preserve">DAVI LOURENZO RODRIGUES PEREIRA</t>
   </si>
   <si>
+    <t xml:space="preserve">DENISE PELEGRINI VERONEZI</t>
+  </si>
+  <si>
     <t xml:space="preserve">EDUARDA KEMILLY OLIVEIRA FARIAS</t>
   </si>
   <si>
@@ -64,6 +76,12 @@
     <t xml:space="preserve">FLAVIA MARIA DOS SANTOS LOPES</t>
   </si>
   <si>
+    <t xml:space="preserve">GLAUCIANE SOUZA MOREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOAO ELI DE SOUZA</t>
+  </si>
+  <si>
     <t xml:space="preserve">JUCILENE DA SILVA C C DOS SANTOS</t>
   </si>
   <si>
@@ -74,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">PEDRO LUCA LOPES COSTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RODRIGO GONCALVES TABOZA</t>
   </si>
   <si>
     <t xml:space="preserve">SILVIA HELENA DE FREITAS RESTINO</t>
@@ -102,7 +123,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -187,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,31 +216,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,8 +307,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,56 +338,89 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>35446</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44490251807</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>3497</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B3" s="3" t="n">
         <v>3621</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>48.76</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>63</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>4644</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="n">
-        <v>50878519831</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>20.87</v>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>4876</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>69</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>3627</v>
+      <c r="A4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>35447</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="2" t="n">
+        <v>40007702841</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>14034</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>4644</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>50878519831</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>3627</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>60405716672</v>
       </c>
-      <c r="E4" s="7" t="n">
-        <v>91.57</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E6" s="4" t="n">
+        <v>9157</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -451,10 +484,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -483,227 +516,311 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="2" t="n">
+        <v>4366</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>35440</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>40251386899</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>5108</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>2006</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B3" s="3" t="n">
         <v>3453</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="8" t="n">
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>25417216844</v>
       </c>
-      <c r="E2" s="9" t="n">
-        <v>169.42</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="E3" s="4" t="n">
+        <v>16942</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>3692</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B4" s="3" t="n">
         <v>3533</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="n">
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="9" t="n">
-        <v>185.7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="E4" s="4" t="n">
+        <v>18570</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>4208</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>15965</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>36258724809</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>23021</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>4365</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B6" s="3" t="n">
         <v>5643</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="8" t="n">
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>51677434864</v>
       </c>
-      <c r="E4" s="9" t="n">
-        <v>111.99</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="E6" s="4" t="n">
+        <v>11199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>4855</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B7" s="3" t="n">
         <v>12530</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="8" t="n">
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>79555772720</v>
       </c>
-      <c r="E5" s="9" t="n">
-        <v>4.66</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+      <c r="E7" s="4" t="n">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
         <v>4748</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B8" s="3" t="n">
         <v>9727</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="8" t="n">
+      <c r="C8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>30049123840</v>
       </c>
-      <c r="E6" s="9" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="n">
+      <c r="E8" s="4" t="n">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>4627</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>35441</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>12008221709</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>4660</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>35442</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>35365494890</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>6311</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
         <v>4100</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B11" s="3" t="n">
         <v>4767</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="8" t="n">
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="n">
         <v>22410014810</v>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E11" s="4" t="n">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>4250</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>4744</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>7815126111</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>17929</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>4509</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>11427</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>53980240860</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>4748</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>9731</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45144859852</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>4052</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>35443</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>35031432896</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>16009</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>4622</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>5625</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>8270231894</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>7913</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>4357</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>3610</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>38844564823</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>4421</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>4836</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>38614238800</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>3176</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>3674</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
-        <v>4250</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>4744</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8" t="n">
-        <v>7815126111</v>
-      </c>
-      <c r="E8" s="9" t="n">
-        <v>179.29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
-        <v>4509</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>11427</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="n">
-        <v>53980240860</v>
-      </c>
-      <c r="E9" s="9" t="n">
-        <v>21.34</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
-        <v>4748</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>9731</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>45144859852</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <v>32.67</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
-        <v>4622</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>5625</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="8" t="n">
-        <v>8270231894</v>
-      </c>
-      <c r="E11" s="9" t="n">
-        <v>79.13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
-        <v>4357</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>3610</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="8" t="n">
-        <v>38844564823</v>
-      </c>
-      <c r="E12" s="9" t="n">
-        <v>21.58</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
-        <v>4421</v>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>4836</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8" t="n">
-        <v>38614238800</v>
-      </c>
-      <c r="E13" s="9" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
-        <v>3176</v>
-      </c>
-      <c r="B14" s="6" t="n">
-        <v>3674</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="8" t="n">
+      <c r="D19" s="2" t="n">
         <v>6581599840</v>
       </c>
-      <c r="E14" s="9" t="n">
-        <v>78.14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E19" s="4" t="n">
+        <v>7814</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>